<commit_message>
aggiornamento attività dic_gen Michele.xlsx
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/SpecificheIndicatori/attività dic_gen Michele.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/SpecificheIndicatori/attività dic_gen Michele.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32000" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="attività dic-gen" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>attività svolte dic/gen</t>
   </si>
@@ -291,9 +291,6 @@
     <t>override va a buon fine</t>
   </si>
   <si>
-    <t>secondo me dovrebbe avere il 12_FL_override = 0 nella logica</t>
-  </si>
-  <si>
     <t>controllo logica BR512</t>
   </si>
   <si>
@@ -310,6 +307,15 @@
   </si>
   <si>
     <t>(dal 221 al 225 Estero)</t>
+  </si>
+  <si>
+    <t>creazione librerie variabili e WS</t>
+  </si>
+  <si>
+    <t>nessun caricamento nell'app</t>
+  </si>
+  <si>
+    <t>secondo me dovrebbe avere il 12_FL_override = 0 nella logica (VEDI SHEET SUCCESSIVA)</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -540,16 +546,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,6 +564,18 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -844,29 +853,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="16" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="10"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
@@ -881,28 +893,28 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>13</v>
       </c>
@@ -915,70 +927,70 @@
       </c>
       <c r="E6" s="22"/>
       <c r="F6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="K7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="18" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
-      <c r="K9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K10" s="2" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K11" s="3"/>
-      <c r="L11" s="2" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I11" s="3"/>
+      <c r="J11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
@@ -988,10 +1000,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>13</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
@@ -1013,7 +1025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
@@ -1055,114 +1067,138 @@
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D22" s="7" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D23" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H24" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D25" s="7" t="s">
+      <c r="A25" s="38">
+        <v>0.8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D27" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="24" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D29" s="7" t="s">
+      <c r="F29" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D31" s="7" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
-        <v>0</v>
-      </c>
-      <c r="D32" t="s">
-        <v>25</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="13">
         <v>0</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="13">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="7" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
+      <c r="G37" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="F29:J29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1216,261 +1252,261 @@
       <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="D12" s="28"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="31"/>
-      <c r="F15" s="31"/>
+      <c r="D15" s="28"/>
+      <c r="F15" s="28"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="29" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="28" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="28" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D25" s="31"/>
-      <c r="F25" s="31"/>
+      <c r="D25" s="28"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="31" t="s">
+      <c r="F27" s="28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D28" s="31"/>
-      <c r="F28" s="31"/>
+      <c r="D28" s="28"/>
+      <c r="F28" s="28"/>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="30" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="29" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D34" s="31"/>
-      <c r="F34" s="31"/>
+      <c r="D34" s="28"/>
+      <c r="F34" s="28"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="D37" s="28"/>
+      <c r="F37" s="28"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D40" s="32" t="s">
+      <c r="D40" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="29" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="28" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D42" s="31" t="s">
+      <c r="D42" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="28" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D43" s="31"/>
-      <c r="F43" s="31"/>
+      <c r="D43" s="28"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D46" s="31"/>
-      <c r="F46" s="31"/>
+      <c r="D46" s="28"/>
+      <c r="F46" s="28"/>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D47" s="35" t="s">
+      <c r="D47" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F47" s="33" t="s">
+      <c r="F47" s="30" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>